<commit_message>
Raspberry Pi update to new software
</commit_message>
<xml_diff>
--- a/Encode_EUI.xlsx
+++ b/Encode_EUI.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="16900" tabRatio="500"/>
+    <workbookView xWindow="580" yWindow="160" windowWidth="25040" windowHeight="16900" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,46 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+  <si>
+    <t>Device EUI</t>
+  </si>
+  <si>
+    <t>00B8C9F8930060F0</t>
+  </si>
+  <si>
+    <t>Application EUI</t>
+  </si>
+  <si>
+    <t>70B3D57ED0022238</t>
+  </si>
+  <si>
+    <t>App Key</t>
+  </si>
+  <si>
+    <t>459777349503CA5FC4AE86BB7A0A2AF8</t>
+  </si>
+  <si>
+    <t>Device Address</t>
+  </si>
+  <si>
+    <t>Network Session Key</t>
+  </si>
+  <si>
+    <t>53C03CFC15FF670A5BD5905CF9C9CAFC</t>
+  </si>
+  <si>
+    <t>App Session Key</t>
+  </si>
+  <si>
+    <t>023A53876F7C5811F6295E4BEEB75EB9</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -48,6 +82,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Consolas"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -66,7 +124,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -90,14 +148,46 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="51">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
@@ -109,6 +199,20 @@
     <cellStyle name="Hipervínculo" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
@@ -120,6 +224,20 @@
     <cellStyle name="Hipervínculo visitado" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -449,7 +567,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:AB7"/>
+  <dimension ref="B5:AB28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
@@ -460,9 +578,9 @@
     <col min="2" max="2" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:28">
-      <c r="B5" s="1">
-        <v>26011348</v>
+    <row r="5" spans="2:28" ht="17">
+      <c r="B5" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:28">
@@ -549,69 +667,69 @@
       </c>
     </row>
     <row r="7" spans="2:28">
-      <c r="B7" t="str">
+      <c r="B7" s="4" t="str">
         <f>CONCATENATE("0x",MID($B5,B6,2),",")</f>
-        <v>0x26,</v>
+        <v>0x02,</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" ref="C7:N7" si="0">CONCATENATE("0x",MID($B5,C6,2),",")</f>
-        <v>0x01,</v>
+        <v>0x3A,</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
-        <v>0x13,</v>
+        <v>0x53,</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
-        <v>0x48,</v>
+        <v>0x87,</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="0"/>
-        <v>0x,</v>
+        <v>0x6F,</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="0"/>
-        <v>0x,</v>
+        <v>0x7C,</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="0"/>
-        <v>0x,</v>
+        <v>0x58,</v>
       </c>
       <c r="I7" t="str">
         <f t="shared" si="0"/>
-        <v>0x,</v>
+        <v>0x11,</v>
       </c>
       <c r="J7" t="str">
         <f t="shared" si="0"/>
-        <v>0x,</v>
+        <v>0xF6,</v>
       </c>
       <c r="K7" t="str">
         <f t="shared" si="0"/>
-        <v>0x,</v>
+        <v>0x29,</v>
       </c>
       <c r="L7" t="str">
         <f t="shared" si="0"/>
-        <v>0x,</v>
+        <v>0x5E,</v>
       </c>
       <c r="M7" t="str">
         <f t="shared" si="0"/>
-        <v>0x,</v>
+        <v>0x4B,</v>
       </c>
       <c r="N7" t="str">
         <f t="shared" si="0"/>
-        <v>0x,</v>
+        <v>0xEE,</v>
       </c>
       <c r="O7" t="str">
         <f t="shared" ref="O7" si="1">CONCATENATE("0x",MID($B5,O6,2),",")</f>
-        <v>0x,</v>
+        <v>0xB7,</v>
       </c>
       <c r="P7" t="str">
         <f t="shared" ref="P7" si="2">CONCATENATE("0x",MID($B5,P6,2),",")</f>
-        <v>0x,</v>
+        <v>0x5E,</v>
       </c>
       <c r="Q7" t="str">
         <f t="shared" ref="Q7" si="3">CONCATENATE("0x",MID($B5,Q6,2),",")</f>
-        <v>0x,</v>
+        <v>0xB9,</v>
       </c>
       <c r="R7" t="str">
         <f t="shared" ref="R7" si="4">CONCATENATE("0x",MID($B5,R6,2),",")</f>
@@ -656,6 +774,66 @@
       <c r="AB7" t="str">
         <f t="shared" ref="AB7" si="14">CONCATENATE("0x",MID($B5,AB6,2),",")</f>
         <v>0x,</v>
+      </c>
+    </row>
+    <row r="12" spans="2:28">
+      <c r="B12" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:28" ht="17">
+      <c r="B13" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:28">
+      <c r="B15" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:28" ht="17">
+      <c r="B16" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" ht="17">
+      <c r="B19" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" ht="17">
+      <c r="B22" s="2">
+        <v>26011297</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" ht="17">
+      <c r="B25" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2">
+      <c r="B27" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" ht="17">
+      <c r="B28" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>